<commit_message>
MPS #comment adiciona funcionalidades de dashboard e cadastro de etecs e alunos etecs
</commit_message>
<xml_diff>
--- a/src/assets/templates/institution.xlsx
+++ b/src/assets/templates/institution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>CODIGO</t>
   </si>
@@ -39,12 +39,6 @@
     <t>São José dos Campos</t>
   </si>
   <si>
-    <t>mentor.a@fatec.sp.gov.br</t>
-  </si>
-  <si>
-    <t>Nome A</t>
-  </si>
-  <si>
     <t>Prof. Jessen Vidal</t>
   </si>
   <si>
@@ -52,6 +46,24 @@
   </si>
   <si>
     <t>Superior</t>
+  </si>
+  <si>
+    <t>Profª Ilza Nascimento Pintus</t>
+  </si>
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Mentor - Fatec</t>
+  </si>
+  <si>
+    <t>Mentor - Etec</t>
+  </si>
+  <si>
+    <t>mentor.etec@etec.sp.gov.br</t>
+  </si>
+  <si>
+    <t>mentor.fatec@fatec.sp.gov.br</t>
   </si>
 </sst>
 </file>
@@ -410,17 +422,17 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -434,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -454,24 +466,43 @@
         <v>31972543000102</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3" s="1">
+        <v>56837222000118</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>

</xml_diff>